<commit_message>
Added simple excel grader functionality.
</commit_message>
<xml_diff>
--- a/config/sample-class/roster.xlsx
+++ b/config/sample-class/roster.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonkuruzovich/githubdesktop/0_class/otter_helper/config/sample-class/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonkuruzovich/GitHub/otter_helper/config/sample-class/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C01C18B-1303-8044-BB1B-F4822AE31E8D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60F8B02-EC6B-6247-BBBF-51F5C8A604A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="920" windowWidth="25040" windowHeight="14280" activeTab="1" xr2:uid="{1EFFBB38-0958-DE43-820D-3F3636858045}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="28">
   <si>
     <t>Username</t>
   </si>
@@ -104,13 +104,19 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>fails4</t>
+  </si>
+  <si>
+    <t>fails3ab</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -462,12 +468,12 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,7 +481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -483,7 +489,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -491,7 +497,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -499,7 +505,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -507,7 +513,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -515,7 +521,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -530,15 +536,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47DB036-F42D-8C49-AD80-27593F80CECB}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="23.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="23.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -573,7 +579,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -593,7 +599,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -613,7 +619,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -633,7 +639,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -653,7 +659,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -673,7 +679,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -690,6 +696,46 @@
         <v>44044.922222222223</v>
       </c>
       <c r="F7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="1">
+        <v>44044.922222222223</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="1">
+        <v>44044.922222222223</v>
+      </c>
+      <c r="F9" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>